<commit_message>
Actualización para U3 (ahora U2) y revisiones
</commit_message>
<xml_diff>
--- a/datos/demografia/barrios.xlsx
+++ b/datos/demografia/barrios.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27425"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Mi unidad\DESVAB - Scripts\data_final\urbanismo\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pablo\Desktop\IEE UPV\DESVAB\datos\demografia\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE1AFF31-8ECF-4512-A8ED-47FD078E96ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EBFB361-4D43-4B10-A5B8-223E6CE46AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -918,12 +940,13 @@
   <dimension ref="A1:H90"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="11" max="11" width="11.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.54296875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
@@ -2795,9 +2818,9 @@
         <f>49495*(D72/SUM($D$72:$D$78))*(1/C72)</f>
         <v>5.3841379919529002</v>
       </c>
-      <c r="H72">
-        <f>G72*(1+0.963936)</f>
-        <v>10.574102431364011</v>
+      <c r="H72" cm="1">
+        <f t="array" ref="H72">G72+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>9.7647711516194811</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -2823,9 +2846,9 @@
         <f t="shared" ref="G73:G78" si="0">49495*(D73/SUM($D$72:$D$78))*(1/C73)</f>
         <v>12.085911111345217</v>
       </c>
-      <c r="H73">
-        <f t="shared" ref="H73:H88" si="1">G73*(1+0.963936)</f>
-        <v>23.735955924370877</v>
+      <c r="H73" cm="1">
+        <f t="array" ref="H73">G73+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>16.466544271011799</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -2851,9 +2874,9 @@
         <f t="shared" si="0"/>
         <v>7.1421149692907662</v>
       </c>
-      <c r="H74">
-        <f t="shared" si="1"/>
-        <v>14.02665670432903</v>
+      <c r="H74" cm="1">
+        <f t="array" ref="H74">G74+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>11.522748128957346</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -2879,9 +2902,9 @@
         <f t="shared" si="0"/>
         <v>13.22236050905825</v>
       </c>
-      <c r="H75">
-        <f t="shared" si="1"/>
-        <v>25.967869808717822</v>
+      <c r="H75" cm="1">
+        <f t="array" ref="H75">G75+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>17.602993668724832</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
@@ -2907,9 +2930,9 @@
         <f t="shared" si="0"/>
         <v>70.441205175948966</v>
       </c>
-      <c r="H76">
-        <f t="shared" si="1"/>
-        <v>138.34201872843249</v>
+      <c r="H76" cm="1">
+        <f t="array" ref="H76">G76+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>74.821838335615553</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
@@ -2935,9 +2958,9 @@
         <f t="shared" si="0"/>
         <v>4.2126796531165516</v>
       </c>
-      <c r="H77">
-        <f t="shared" si="1"/>
-        <v>8.2734332272231068</v>
+      <c r="H77" cm="1">
+        <f t="array" ref="H77">G77+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>8.5933128127831324</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
@@ -2963,9 +2986,9 @@
         <f t="shared" si="0"/>
         <v>7.2617785056697892</v>
       </c>
-      <c r="H78">
-        <f t="shared" si="1"/>
-        <v>14.261668231311102</v>
+      <c r="H78" cm="1">
+        <f t="array" ref="H78">G78+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>11.64241166533637</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -2991,9 +3014,9 @@
         <f>85943*(D79/SUM($D$79:$D$80))*(1/C79)</f>
         <v>4.7196702707433511</v>
       </c>
-      <c r="H79">
-        <f t="shared" si="1"/>
-        <v>9.2691303528426143</v>
+      <c r="H79" cm="1">
+        <f t="array" ref="H79">G79+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>9.1003034304099319</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -3019,9 +3042,9 @@
         <f>85943*(D80/SUM($D$79:$D$80))*(1/C80)</f>
         <v>19.4854057462064</v>
       </c>
-      <c r="H80">
-        <f t="shared" si="1"/>
-        <v>38.268089819581611</v>
+      <c r="H80" cm="1">
+        <f t="array" ref="H80">G80+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>23.86603890587298</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -3047,9 +3070,9 @@
         <f>100236*(D81/SUM($D$81:$D$88))*(1/C81)</f>
         <v>2.897858508914831</v>
       </c>
-      <c r="H81">
-        <f t="shared" si="1"/>
-        <v>5.6912086485641575</v>
+      <c r="H81" cm="1">
+        <f t="array" ref="H81">G81+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>7.2784916685814114</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -3072,12 +3095,12 @@
         <v>30187.8458136792</v>
       </c>
       <c r="G82">
-        <f t="shared" ref="G82:G88" si="2">100236*(D82/SUM($D$81:$D$88))*(1/C82)</f>
+        <f t="shared" ref="G82:G88" si="1">100236*(D82/SUM($D$81:$D$88))*(1/C82)</f>
         <v>1.3594903155622773</v>
       </c>
-      <c r="H82">
-        <f t="shared" si="1"/>
-        <v>2.6699519723841165</v>
+      <c r="H82" cm="1">
+        <f t="array" ref="H82">G82+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>5.7401234752288577</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -3100,12 +3123,12 @@
         <v>31968.629499217499</v>
       </c>
       <c r="G83">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>7.7684236106531088</v>
       </c>
-      <c r="H83">
-        <f t="shared" si="1"/>
-        <v>15.256686792211623</v>
+      <c r="H83" cm="1">
+        <f t="array" ref="H83">G83+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>12.149056770319689</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
@@ -3128,12 +3151,12 @@
         <v>37668</v>
       </c>
       <c r="G84">
-        <f t="shared" si="2"/>
+        <f>100236*(D84/SUM($D$81:$D$88))*(1/C84)</f>
         <v>13.453632919331175</v>
       </c>
-      <c r="H84">
-        <f t="shared" si="1"/>
-        <v>26.42207402105959</v>
+      <c r="H84" cm="1">
+        <f t="array" ref="H84">G84+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>17.834266078997757</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
@@ -3156,12 +3179,12 @@
         <v>34658</v>
       </c>
       <c r="G85">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>13.011076207025777</v>
       </c>
-      <c r="H85">
-        <f t="shared" si="1"/>
-        <v>25.552920961721377</v>
+      <c r="H85" cm="1">
+        <f t="array" ref="H85">G85+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>17.391709366692357</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
@@ -3184,12 +3207,12 @@
         <v>33927</v>
       </c>
       <c r="G86">
-        <f t="shared" si="2"/>
+        <f>100236*(D86/SUM($D$81:$D$88))*(1/C86)</f>
         <v>10.237781217407466</v>
       </c>
-      <c r="H86">
-        <f t="shared" si="1"/>
-        <v>20.106347092990347</v>
+      <c r="H86" cm="1">
+        <f t="array" ref="H86">G86+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>14.618414377074046</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -3215,9 +3238,9 @@
         <f>100236*(D87/SUM($D$81:$D$88))*(1/C87)</f>
         <v>0.26587489315548146</v>
       </c>
-      <c r="H87">
-        <f t="shared" si="1"/>
-        <v>0.52216127416420366</v>
+      <c r="H87" cm="1">
+        <f t="array" ref="H87">G87+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>4.6465080528220621</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -3240,12 +3263,12 @@
         <v>23492</v>
       </c>
       <c r="G88">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>9.537187073388063</v>
       </c>
-      <c r="H88">
-        <f t="shared" si="1"/>
-        <v>18.73042503216146</v>
+      <c r="H88" cm="1">
+        <f t="array" ref="H88">G88+SUM(($H$2:$H$71 - $G$2:$G$71) * $C$2:$C$71) / SUM($C$2:$C$71)</f>
+        <v>13.917820233054645</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>